<commit_message>
update the region & gender
add TT-1st Mile two Vice-Chair
</commit_message>
<xml_diff>
--- a/SC-IMT ET TT Overview.xlsx
+++ b/SC-IMT ET TT Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wmoomm-my.sharepoint.com/personal/xchen_wmo_int/Documents/Documents/chenxx/work/WMO/2024/SC-IMT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="199" documentId="8_{A6073DA9-5548-495D-A94C-24ABCE89EE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94027D32-DD3A-4CE8-8F9B-F3BDDF97D090}"/>
+  <xr:revisionPtr revIDLastSave="236" documentId="8_{A6073DA9-5548-495D-A94C-24ABCE89EE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0ABB5439-F838-4D54-AC6C-754BCB3EA815}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F92D2B54-C5C5-4016-B51D-B66DCB2F1504}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="59">
   <si>
     <t>Information Systems</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Chair</t>
   </si>
   <si>
-    <t>Vice-Chair</t>
-  </si>
-  <si>
     <t>Jeremy Tandy</t>
   </si>
   <si>
@@ -254,9 +251,6 @@
     <t>Büßelberg Thorsten</t>
   </si>
   <si>
-    <t>Eugene Burger</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -336,6 +330,21 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Eugene Burger*</t>
+  </si>
+  <si>
+    <t>Co-Chair/Vice-Chair*</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Douglas Body*</t>
+  </si>
+  <si>
+    <t>Ilse Gayl*</t>
   </si>
 </sst>
 </file>
@@ -474,36 +483,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -518,20 +509,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -551,6 +530,48 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,7 +680,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'SC-IMT'!$B$16</c:f>
+              <c:f>'SC-IMT'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -737,7 +758,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'SC-IMT'!$A$17:$A$22</c:f>
+              <c:f>'SC-IMT'!$A$18:$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -763,7 +784,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SC-IMT'!$B$17:$B$22</c:f>
+              <c:f>'SC-IMT'!$B$18:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -777,10 +798,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
@@ -1056,7 +1077,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'SC-IMT'!$B$25</c:f>
+              <c:f>'SC-IMT'!$B$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1192,7 +1213,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'SC-IMT'!$A$26:$A$27</c:f>
+              <c:f>'SC-IMT'!$A$27:$A$28</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1206,15 +1227,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'SC-IMT'!$B$26:$B$27</c:f>
+              <c:f>'SC-IMT'!$B$27:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2424,13 +2445,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>150812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>173037</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2460,13 +2481,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>93662</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3552825</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>115887</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2792,10 +2813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F11A09-FF77-4E3D-B40E-BA7295BF033A}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2810,432 +2831,465 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="D2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>33</v>
+      <c r="H2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="12" t="s">
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>50</v>
+      <c r="F3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>51</v>
+      <c r="I4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="21"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="25"/>
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>50</v>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="21"/>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="21"/>
+      <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="25"/>
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="21"/>
+      <c r="C9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="21"/>
+      <c r="C10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="21"/>
+      <c r="C11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="25"/>
+      <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="I12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="25"/>
+      <c r="B13" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="15" t="s">
+      <c r="C13" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="25"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="23"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>54</v>
+      <c r="I14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="28">
-        <v>1</v>
+      <c r="A17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="28">
-        <v>2</v>
+      <c r="B18" s="18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="28">
-        <v>0</v>
+      <c r="A19" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="18">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="28">
-        <v>4</v>
+      <c r="A20" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="18">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="28">
-        <v>0</v>
+      <c r="A21" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="18">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="28">
-        <v>6</v>
+      <c r="A22" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="18">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="30">
+      <c r="A23" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="20">
         <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="13">
-        <v>8</v>
+      <c r="A26" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="16">
-        <v>5</v>
+      <c r="A27" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="9">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="12">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>